<commit_message>
Fix: Handles if specific value is empty
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RPA\Theresia\RPA-ManadskollArvoderadeUppdrag\RPA-ManadskollArvoderadeUppdrag inte i git\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RPA\Theresia\RPA-Kontroll-Av-Utanordningslista\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450" activeTab="2"/>
+    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>ExScreenshotsFolderPath</t>
-  </si>
-  <si>
-    <t>Exceptions_Screenshots</t>
   </si>
   <si>
     <t>Where to save exceptions screenshots - can be a full or a relative path.</t>
@@ -201,13 +198,19 @@
   </si>
   <si>
     <t>ProcapitaRole</t>
+  </si>
+  <si>
+    <t>\\safs008\RPA\VoF\RPA_030\Temp</t>
+  </si>
+  <si>
+    <t>TRUE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -231,6 +234,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -249,10 +258,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -262,8 +272,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlänk" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -626,50 +638,50 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1673,8 +1685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1727,29 +1739,29 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="30">
       <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1757,113 +1769,113 @@
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
         <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
         <v>18</v>
       </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:3" ht="45">
       <c r="A18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" t="b">
-        <v>0</v>
+        <v>39</v>
+      </c>
+      <c r="B18" t="s">
+        <v>59</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2839,6 +2851,9 @@
     <row r="989" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2847,7 +2862,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -2867,7 +2882,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2897,77 +2912,77 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
         <v>44</v>
-      </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Fix: Splittied Asset for PercentToAcceptUtanordningslistanArvode, PercentToAcceptUtanordningslistanOmkostnad
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450" activeTab="1"/>
+    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -204,6 +204,12 @@
   </si>
   <si>
     <t>TRUE</t>
+  </si>
+  <si>
+    <t>PercentToAcceptUtanordningslistanArvode</t>
+  </si>
+  <si>
+    <t>PercentToAcceptUtanordningslistanOmkostnad</t>
   </si>
 </sst>
 </file>
@@ -1685,7 +1691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -2860,10 +2866,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2958,7 +2964,7 @@
         <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1">
@@ -2985,7 +2991,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3973,7 +3986,6 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix: Only check if arvode is ok.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450" activeTab="2"/>
+    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -1691,8 +1691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1753,7 +1753,7 @@
         <v>32</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>40</v>
@@ -2868,7 +2868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix: Renames file when done.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450" activeTab="1"/>
+    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -210,6 +207,21 @@
   </si>
   <si>
     <t>PercentToAcceptUtanordningslistanOmkostnad</t>
+  </si>
+  <si>
+    <t>Kontroll av utanordningslista</t>
+  </si>
+  <si>
+    <t>ProcessingPrefix</t>
+  </si>
+  <si>
+    <t>_Hanteras</t>
+  </si>
+  <si>
+    <t>FinishedPrefix</t>
+  </si>
+  <si>
+    <t>_Klar</t>
   </si>
 </sst>
 </file>
@@ -596,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -644,22 +656,22 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -668,30 +680,44 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" t="s">
+        <v>65</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1691,7 +1717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1745,29 +1771,29 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="30">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1776,7 +1802,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -1791,7 +1817,7 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -1813,7 +1839,7 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1824,7 +1850,7 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -1835,53 +1861,53 @@
         <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:3" ht="45">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2869,12 +2895,12 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="1" max="1" width="45.140625" customWidth="1"/>
     <col min="2" max="2" width="30.140625" customWidth="1"/>
     <col min="3" max="3" width="60.28515625" customWidth="1"/>
     <col min="4" max="26" width="65.42578125" customWidth="1"/>
@@ -2888,7 +2914,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2918,85 +2944,85 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
         <v>43</v>
-      </c>
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>